<commit_message>
NC92Soil - Versione 0.8 bis del 08/10/2020
- Implementata generazione dei file di input batch per l'analisi a permutazione
- Implementata possibilità di definire leggi di variazioni custom per la Vs dei terreni in funzione della profondità
- Implementata possibilità di aggiungere automaticamente il bedrock geologico fino al raggiungimento della velocità di 800 m/s
</commit_message>
<xml_diff>
--- a/Stochastic input 2.xlsx
+++ b/Stochastic input 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaac\Documents\Repo Git\GitLab\SRA Software\GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48A1946-F8AF-45D2-AD04-900604A6D189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DF3540-5741-44C5-9725-B442B20568EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4D2D38F4-E5D1-49A1-97A0-EF49BC19DD52}"/>
   </bookViews>
@@ -174,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>Unit weight
 [KN/m3]</t>
@@ -248,9 +248,6 @@
 [m]</t>
   </si>
   <si>
-    <t>2*G + G^0.25 + 3; G - G^0.6 + 10</t>
-  </si>
-  <si>
     <t>Bedrock Vs
 [m/s]</t>
   </si>
@@ -277,6 +274,22 @@
   </si>
   <si>
     <t>150.29*H^0.17+0.03</t>
+  </si>
+  <si>
+    <t>2*G + G^0.25 + 3; D - D^0.6 + 10</t>
+  </si>
+  <si>
+    <t>Analys type</t>
+  </si>
+  <si>
+    <t>Permutations</t>
+  </si>
+  <si>
+    <t>MOPS</t>
+  </si>
+  <si>
+    <t>Brick size
+[m]</t>
   </si>
 </sst>
 </file>
@@ -354,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -371,6 +384,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -688,7 +704,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,7 +766,7 @@
         <v>20</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="7">
         <v>0.39</v>
@@ -759,7 +775,7 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="I2">
         <v>28</v>
@@ -782,7 +798,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="7">
         <v>0.44</v>
@@ -802,7 +818,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>18</v>
@@ -814,7 +830,7 @@
         <v>20</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="7">
         <v>0.38</v>
@@ -834,7 +850,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>18</v>
@@ -846,7 +862,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="7">
         <v>0.39</v>
@@ -866,7 +882,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>18</v>
@@ -878,7 +894,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="7">
         <v>0.4</v>
@@ -904,10 +920,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4957287E-A37F-4CE2-B169-A739F2ED3546}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -920,16 +936,17 @@
     <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="16.5546875" customWidth="1"/>
     <col min="11" max="11" width="16.5546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="2.6640625" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" customWidth="1"/>
     <col min="13" max="13" width="5.5546875" customWidth="1"/>
     <col min="14" max="14" width="3.5546875" customWidth="1"/>
     <col min="15" max="15" width="19.5546875" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -962,6 +979,9 @@
       <c r="K1" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="L1" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="O1" s="4" t="s">
         <v>8</v>
       </c>
@@ -972,18 +992,27 @@
         <v>14</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
       <c r="O2">
-        <v>3</v>
+        <v>200</v>
+      </c>
+      <c r="P2">
+        <v>7</v>
       </c>
       <c r="Q2" t="s">
         <v>15</v>
@@ -991,8 +1020,11 @@
       <c r="R2">
         <v>400</v>
       </c>
+      <c r="S2" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1000,12 +1032,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1015,12 +1047,18 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F68390BF-BE40-4FA6-8740-D490E73B4B13}">
           <x14:formula1>
             <xm:f>Voices!$A$1:$A$2</xm:f>
           </x14:formula1>
           <xm:sqref>Q2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BF99A6F8-3247-4991-A1B9-375B041DD545}">
+          <x14:formula1>
+            <xm:f>Voices!$C$1:$C$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>S2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1030,25 +1068,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749CBBA9-59D3-4962-B318-181DD931EBB9}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>